<commit_message>
update recon example (#8)
Co-authored-by: Stephen LM <stephen.lemasney@finbourne.com>
</commit_message>
<xml_diff>
--- a/examples/lusid/run-a-reconciliation/_data/equity_holdings_20220301.xlsx
+++ b/examples/lusid/run-a-reconciliation/_data/equity_holdings_20220301.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\code\gl\luminesce-examples\examples\lusid\run-a-reconcilation\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\code\gl\luminesce-examples\examples\lusid\run-a-reconciliation\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55A1C20-05E5-4984-87FC-D5A1AC30F5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21396B32-0A8E-4B35-806B-2BEDD8A91259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lusid_holdings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="147">
   <si>
     <t>InstrumentId</t>
   </si>
@@ -465,6 +465,9 @@
   </si>
   <si>
     <t>currency</t>
+  </si>
+  <si>
+    <t>UkEquityActive</t>
   </si>
 </sst>
 </file>
@@ -783,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A11:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -794,7 +797,7 @@
     <col min="1" max="1" width="13.734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.9453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.3671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.47265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -964,6 +967,91 @@
         <v>240</v>
       </c>
       <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11">
+        <v>1000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12">
+        <v>2000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>1500</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14">
+        <v>1000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15">
+        <v>1750</v>
+      </c>
+      <c r="E15" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1687,14 +1775,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C142B5-16CD-4229-9C5D-A5183069E561}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="13.734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.9453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.3671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1869,6 +1958,91 @@
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11">
+        <v>1000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12">
+        <v>2000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>1500</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14">
+        <v>1000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15">
+        <v>1750</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>